<commit_message>
Adding percentage data to Lab 13 and fixing an error with Lab 14
</commit_message>
<xml_diff>
--- a/13_changes_in_salt_intake/13_changes_in_salt_intake_data.xlsx
+++ b/13_changes_in_salt_intake/13_changes_in_salt_intake_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="14">
   <si>
     <t>Salt Variance with AngII</t>
   </si>
@@ -53,12 +53,18 @@
   <si>
     <t>QCP</t>
   </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +78,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -81,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -141,24 +154,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -175,20 +176,98 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -478,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:I20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -496,6 +575,9 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -513,13 +595,13 @@
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="9">
         <v>20</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="9">
         <v>180</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="9">
         <v>500</v>
       </c>
     </row>
@@ -536,16 +618,16 @@
       <c r="D3" s="4">
         <v>99</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>77</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="1">
         <v>88</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>91</v>
       </c>
     </row>
@@ -562,16 +644,16 @@
       <c r="D4" s="4">
         <v>0.4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>-1.5</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
         <v>-0.3</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>0.1</v>
       </c>
     </row>
@@ -588,16 +670,16 @@
       <c r="D5" s="4">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>0.7</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="1">
         <v>2.8</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="1">
         <v>3.5</v>
       </c>
     </row>
@@ -614,16 +696,16 @@
       <c r="D6" s="4">
         <v>13</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>0</v>
       </c>
     </row>
@@ -640,16 +722,16 @@
       <c r="D7" s="4">
         <v>183</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>327</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>181</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>139</v>
       </c>
     </row>
@@ -666,16 +748,16 @@
       <c r="D8" s="4">
         <v>21</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>7</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>15</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>18</v>
       </c>
     </row>
@@ -692,27 +774,30 @@
       <c r="D9" s="4">
         <v>0.35299999999999998</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="1">
         <v>0.121</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="1">
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+    <row r="10" spans="1:9">
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" ht="30.75" thickBot="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -911,36 +996,305 @@
       <c r="D19" s="4">
         <v>0.35899999999999999</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="1">
         <v>2.3E-2</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="1">
         <v>0.125</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="1">
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+    <row r="20" spans="1:9">
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30.75" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2">
+        <v>180</v>
+      </c>
+      <c r="D23" s="2">
+        <v>500</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9">
+        <v>20</v>
+      </c>
+      <c r="H23" s="9">
+        <v>180</v>
+      </c>
+      <c r="I23" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="60.75" thickBot="1">
+      <c r="A24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="10">
+        <f>ABS((B3-B13)/B3)</f>
+        <v>3.5106382978723372E-2</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" ref="C24:D24" si="0">ABS((C3-C13)/C3)</f>
+        <v>4.1237113402062438E-3</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="0"/>
+        <v>2.1212121212121154E-2</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="10">
+        <f>ABS((G3-G13)/G3)</f>
+        <v>0.10129870129870126</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" ref="H24:I24" si="1">ABS((H3-H13)/H3)</f>
+        <v>1.1363636363636364E-2</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="1"/>
+        <v>1.0989010989010365E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="75.75" thickBot="1">
+      <c r="A25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10">
+        <f t="shared" ref="B25:D25" si="2">ABS((B4-B14)/B4)</f>
+        <v>1.2</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" si="2"/>
+        <v>10.999999999999998</v>
+      </c>
+      <c r="D25" s="10">
+        <f t="shared" si="2"/>
+        <v>4.25</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="10">
+        <f t="shared" ref="G25:I25" si="3">ABS((G4-G14)/G4)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="75.75" thickBot="1">
+      <c r="A26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="10">
+        <f t="shared" ref="B26:D26" si="4">ABS((B5-B15)/B5)</f>
+        <v>0.70833333333333326</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="4"/>
+        <v>0.48571428571428577</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" si="4"/>
+        <v>0.48780487804878053</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="10">
+        <f t="shared" ref="G26:I26" si="5">ABS((G5-G15)/G5)</f>
+        <v>1.8571428571428574</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="5"/>
+        <v>0.42857142857142866</v>
+      </c>
+      <c r="I26" s="10">
+        <f t="shared" si="5"/>
+        <v>0.45714285714285702</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45.75" thickBot="1">
+      <c r="A27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="10">
+        <f t="shared" ref="B27:D27" si="6">ABS((B6-B16)/B6)</f>
+        <v>3.8095238095238126E-2</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="6"/>
+        <v>0.11500000000000003</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="6"/>
+        <v>9.2307692307692257E-2</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="60.75" thickBot="1">
+      <c r="A28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="10">
+        <f t="shared" ref="B28:D28" si="7">ABS((B7-B17)/B7)</f>
+        <v>0.18923556942277683</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="7"/>
+        <v>5.1027397260273895E-2</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="7"/>
+        <v>0.17540983606557373</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="10">
+        <f t="shared" ref="G28:I28" si="8">ABS((G7-G17)/G7)</f>
+        <v>0.23608562691131496</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="8"/>
+        <v>9.3922651933701033E-3</v>
+      </c>
+      <c r="I28" s="10">
+        <f t="shared" si="8"/>
+        <v>5.0359712230215826E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45.75" thickBot="1">
+      <c r="A29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="10">
+        <f t="shared" ref="B29:D29" si="9">ABS((B8-B18)/B8)</f>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="C29" s="10">
+        <f t="shared" si="9"/>
+        <v>0.24444444444444435</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" si="9"/>
+        <v>0.18095238095238098</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="10">
+        <f t="shared" ref="G29:I29" si="10">ABS((G8-G18)/G8)</f>
+        <v>1.0142857142857142</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="10"/>
+        <v>0.45999999999999991</v>
+      </c>
+      <c r="I29" s="10">
+        <f t="shared" si="10"/>
+        <v>0.3888888888888889</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="75.75" thickBot="1">
+      <c r="A30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="10">
+        <f t="shared" ref="B30:D30" si="11">ABS((B9-B19)/B9)</f>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="C30" s="10">
+        <f t="shared" si="11"/>
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="11"/>
+        <v>1.6997167138810214E-2</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="10">
+        <f t="shared" ref="G30:I30" si="12">ABS((G9-G19)/G9)</f>
+        <v>1.5555555555555558</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="12"/>
+        <v>3.305785123966945E-2</v>
+      </c>
+      <c r="I30" s="10">
+        <f t="shared" si="12"/>
+        <v>2.9154518950437343E-3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-  </mergeCells>
+  <conditionalFormatting sqref="B24:D30">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24:I30">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>